<commit_message>
WIP Import work area
</commit_message>
<xml_diff>
--- a/storage/app/import/work-areas.xlsx
+++ b/storage/app/import/work-areas.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkukuh/code/memfis/storage/app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\MeMFIS\storage\app\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5074954B-1185-442E-B355-E9BA3D82BB55}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
   <si>
     <t>AC DIST BAY</t>
   </si>
@@ -396,13 +397,157 @@
   </si>
   <si>
     <t>WING RH</t>
+  </si>
+  <si>
+    <t>MAIN LANDING GEAR</t>
+  </si>
+  <si>
+    <t>WING</t>
+  </si>
+  <si>
+    <t>DOOR</t>
+  </si>
+  <si>
+    <t>STABILIZER</t>
+  </si>
+  <si>
+    <t>HORIZONTAL STABILIZER</t>
+  </si>
+  <si>
+    <t>DOOR SYSTEM</t>
+  </si>
+  <si>
+    <t>COCKPIT</t>
+  </si>
+  <si>
+    <t>CABIN MAINTENANCE</t>
+  </si>
+  <si>
+    <t>PASS COMPARTMENT</t>
+  </si>
+  <si>
+    <t>CABIN MAINTENANCE PASSANGERS</t>
+  </si>
+  <si>
+    <t>EMEPENAGE</t>
+  </si>
+  <si>
+    <t>CENTER WING</t>
+  </si>
+  <si>
+    <t>FLIGHT COMPARTMENT</t>
+  </si>
+  <si>
+    <t>DORSAL FIN</t>
+  </si>
+  <si>
+    <t>FUEL TANK</t>
+  </si>
+  <si>
+    <t>MAIN FUEL TANK</t>
+  </si>
+  <si>
+    <t>EMERGENCY EXIT DOOR</t>
+  </si>
+  <si>
+    <t>PASS CABIN MAINTENANCE</t>
+  </si>
+  <si>
+    <t>PASS DOOR</t>
+  </si>
+  <si>
+    <t>RADIO RACK</t>
+  </si>
+  <si>
+    <t>UPPER FUSELAGE</t>
+  </si>
+  <si>
+    <t>NOSE WHEEL WELL</t>
+  </si>
+  <si>
+    <t>NOSE LANG GEAR</t>
+  </si>
+  <si>
+    <t>LOWER HALF OF FUSELAGE - EXTERNAL</t>
+  </si>
+  <si>
+    <t>RADOME/NOSE FUSELAGE – INTERNAL</t>
+  </si>
+  <si>
+    <t>PRESSURIZED ZONE UNDER PILOT / COPILOT FLOOR – INTERNAL</t>
+  </si>
+  <si>
+    <t>COMPARTMENT UNDER MAIN CABIN FLOOR – INTERNAL</t>
+  </si>
+  <si>
+    <t>FUSELAGE – FLIGHT CREW COMPARTMENT</t>
+  </si>
+  <si>
+    <t>FUSELAGE – CABIN COMPARTMENT</t>
+  </si>
+  <si>
+    <t>REAR FUSELAGE FROM FRAMES 30 TO 46 - INTERNAL</t>
+  </si>
+  <si>
+    <t>REAR FUSELAGE FROM FRAMES 30 TO 46 - EXTERNAL</t>
+  </si>
+  <si>
+    <t>FUSELAGE TAIL SECTION</t>
+  </si>
+  <si>
+    <t>FUSELAGE – UNDER WING TO BODY FAIRING</t>
+  </si>
+  <si>
+    <t>VERTICAL STABILIZER MAIN BOX - INTERNAL</t>
+  </si>
+  <si>
+    <t>VERTICAL STABILIZER - EXTERNAL</t>
+  </si>
+  <si>
+    <t>VERTICAL STABILIZER TRAILING EDGE - INTERNAL</t>
+  </si>
+  <si>
+    <t>HORIZONTAL STABILIZER TRAILING EDGE - INTERNAL</t>
+  </si>
+  <si>
+    <t>HORIZONTAL STABILIZER - EXTERNAL</t>
+  </si>
+  <si>
+    <t>HORIZONTAL STABILIZER SPAR BOX - INTERNAL</t>
+  </si>
+  <si>
+    <t>HORIZONTAL STABILIZER LEADING EDGE - INTERNAL</t>
+  </si>
+  <si>
+    <t>VERTICAL STABILIZER LEADING EDGE - INTERNAL</t>
+  </si>
+  <si>
+    <t>OUTER WING AND FLAPS – EXTERNAL</t>
+  </si>
+  <si>
+    <t>OUTER WING SPAR BOX – INTERNAL</t>
+  </si>
+  <si>
+    <t>OUTER WING TRAILING EDGES AND FLAPS - INTERNAL</t>
+  </si>
+  <si>
+    <t>CENTER WING – EXTERNAL</t>
+  </si>
+  <si>
+    <t>CENTER WING  - SPAR BOX (FUEL TANK)</t>
+  </si>
+  <si>
+    <t>CENTER WING TRAILING EDGES AND FLAPS - INTERNAL</t>
+  </si>
+  <si>
+    <t>POWER PLANT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -410,16 +555,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -427,21 +596,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 17" xfId="2" xr:uid="{22FC9792-ED2C-40D4-AB1E-CFED13FE466F}"/>
+    <cellStyle name="Normal 26" xfId="1" xr:uid="{EBE2B4E5-8FC2-4193-A8B4-43634F4C88E8}"/>
+    <cellStyle name="Normal 27" xfId="3" xr:uid="{4D11351D-9FEF-449B-8337-0954DB64165A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -709,634 +941,877 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A123"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E176" sqref="E176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="42" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="93" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+    <row r="111" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A119" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+    <row r="162" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:A171">
+    <sortCondition ref="A124"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Support encoding utf8mb4 character
</commit_message>
<xml_diff>
--- a/storage/app/import/work-areas.xlsx
+++ b/storage/app/import/work-areas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\MeMFIS\storage\app\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkukuh/Sites/memfis/storage/app/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5074954B-1185-442E-B355-E9BA3D82BB55}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A7084E-C22B-E545-8213-31A517878418}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,21 +471,6 @@
     <t>LOWER HALF OF FUSELAGE - EXTERNAL</t>
   </si>
   <si>
-    <t>RADOME/NOSE FUSELAGE – INTERNAL</t>
-  </si>
-  <si>
-    <t>PRESSURIZED ZONE UNDER PILOT / COPILOT FLOOR – INTERNAL</t>
-  </si>
-  <si>
-    <t>COMPARTMENT UNDER MAIN CABIN FLOOR – INTERNAL</t>
-  </si>
-  <si>
-    <t>FUSELAGE – FLIGHT CREW COMPARTMENT</t>
-  </si>
-  <si>
-    <t>FUSELAGE – CABIN COMPARTMENT</t>
-  </si>
-  <si>
     <t>REAR FUSELAGE FROM FRAMES 30 TO 46 - INTERNAL</t>
   </si>
   <si>
@@ -495,9 +480,6 @@
     <t>FUSELAGE TAIL SECTION</t>
   </si>
   <si>
-    <t>FUSELAGE – UNDER WING TO BODY FAIRING</t>
-  </si>
-  <si>
     <t>VERTICAL STABILIZER MAIN BOX - INTERNAL</t>
   </si>
   <si>
@@ -522,18 +504,9 @@
     <t>VERTICAL STABILIZER LEADING EDGE - INTERNAL</t>
   </si>
   <si>
-    <t>OUTER WING AND FLAPS – EXTERNAL</t>
-  </si>
-  <si>
-    <t>OUTER WING SPAR BOX – INTERNAL</t>
-  </si>
-  <si>
     <t>OUTER WING TRAILING EDGES AND FLAPS - INTERNAL</t>
   </si>
   <si>
-    <t>CENTER WING – EXTERNAL</t>
-  </si>
-  <si>
     <t>CENTER WING  - SPAR BOX (FUEL TANK)</t>
   </si>
   <si>
@@ -541,6 +514,33 @@
   </si>
   <si>
     <t>POWER PLANT</t>
+  </si>
+  <si>
+    <t>CENTER WING - EXTERNAL</t>
+  </si>
+  <si>
+    <t>COMPARTMENT UNDER MAIN CABIN FLOOR - INTERNAL</t>
+  </si>
+  <si>
+    <t>FUSELAGE - CABIN COMPARTMENT</t>
+  </si>
+  <si>
+    <t>FUSELAGE - FLIGHT CREW COMPARTMENT</t>
+  </si>
+  <si>
+    <t>FUSELAGE - UNDER WING TO BODY FAIRING</t>
+  </si>
+  <si>
+    <t>OUTER WING AND FLAPS - EXTERNAL</t>
+  </si>
+  <si>
+    <t>OUTER WING SPAR BOX - INTERNAL</t>
+  </si>
+  <si>
+    <t>PRESSURIZED ZONE UNDER PILOT / COPILOT FLOOR - INTERNAL</t>
+  </si>
+  <si>
+    <t>RADOME/NOSE FUSELAGE - INTERNAL</t>
   </si>
 </sst>
 </file>
@@ -944,872 +944,872 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E176" sqref="E176"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="K102" sqref="K102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" ht="48" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A127" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A128" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A127" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="162" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A163" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="163" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" s="5" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A171">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A171">
     <sortCondition ref="A124"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>